<commit_message>
Development Center in Extension
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.menu.xlsx
+++ b/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/ambient.menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/Develop/Source/ox-workshop/vertx-zero/vertx-pin/zero-ambient/src/main/resources/plugin/ambient/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0FC0D1-9628-6D4A-9C9C-18B88F438BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBC6875-5D97-D544-9833-AB7B29B4E1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54340" yWindow="-3520" windowWidth="38400" windowHeight="22620" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
+    <workbookView xWindow="43640" yWindow="-6020" windowWidth="43440" windowHeight="22660" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA-MENU" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="188">
   <si>
     <t>name</t>
   </si>
@@ -232,10 +232,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>zero.system.file</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>文件管理</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -262,9 +258,6 @@
     <t>字典管理</t>
   </si>
   <si>
-    <t>/acme/tabular</t>
-  </si>
-  <si>
     <t>ef010bf1-3e4d-4727-9ef4-ba5b81b5a1c2</t>
   </si>
   <si>
@@ -274,17 +267,6 @@
     <t>cluster</t>
   </si>
   <si>
-    <t>/acme/category</t>
-  </si>
-  <si>
-    <t>zero.epic.metadata</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>zero.epic.category</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>66c86ff3-39fe-4fbb-8bb4-8b8977b9745b</t>
   </si>
   <si>
@@ -300,74 +282,20 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>12b5f844-66b6-4034-b717-9d3224c7fb65</t>
-  </si>
-  <si>
-    <t>zero.data.system</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>系统数据</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EXPAND</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>SIDE-MENU</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>开发中心</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>c7cfa352-0b7f-4b1d-91ba-8de91468ee4c</t>
   </si>
   <si>
-    <t>0d8d516f-429f-421a-a23d-b4b364dad951</t>
-  </si>
-  <si>
     <t>ee635f66-62f6-4f16-b1ca-7fa1c0ee06b9</t>
   </si>
   <si>
-    <t>zero.develop</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>zero.develop.workflow</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>zero.develop.report</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>流程设计</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>branches</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>报表设计</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>area-chart</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>/epic/workflow</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>/epic/report</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>模块参数</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -384,10 +312,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>environment</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>全局配置</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -407,18 +331,6 @@
     <t>1aa58879-1125-429a-b485-bfbbcc55ebde</t>
   </si>
   <si>
-    <t>文件存储</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/system/file-store</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>zero.system.file-store</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>日志管理</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -447,10 +359,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cloud-upload</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>file-add</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -463,9 +371,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>07fe771a-712d-466e-b22e-1616a04e94e4</t>
-  </si>
-  <si>
     <t>b09c258a-d737-492a-8766-5092bcd31d4b</t>
   </si>
   <si>
@@ -473,14 +378,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>zero.system.file-my</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/system/file-my</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>各种审批</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -511,37 +408,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>文件流程</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>file</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>zero.system.file-w</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>zero.system.file-w.done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>zero.system.file-w.open</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>zero.system.file-w.approval</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>audit</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>fe6e15c5-18b8-403d-a7f3-83c39f36ffc1</t>
-  </si>
-  <si>
     <t>0a902f35-a4fd-425a-9a1a-c15bf3fa345f</t>
   </si>
   <si>
@@ -619,6 +493,218 @@
   </si>
   <si>
     <t>个人报表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>文件类型</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ambient/category/zero.file.tree</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0ca01825-953f-46bc-ae27-9dae317a2b82</t>
+  </si>
+  <si>
+    <t>平台应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DEV-MENU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop.app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>appstore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>应用设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop.app.setting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop.app.data-source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数据源</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/application/setting</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/application/database</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop.app.module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模块管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>database</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deployment-unit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/application/module</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop.app.module-config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>模块配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/application/module-config</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop.app.menu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>菜单管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>menu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/application/menu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ab07e5df-94ac-43c0-a66d-55131627ee33</t>
+  </si>
+  <si>
+    <t>1f71c9c4-4d01-46de-8105-9d44d633678b</t>
+  </si>
+  <si>
+    <t>a8f56c74-4215-4e98-86bb-1293787d5db6</t>
+  </si>
+  <si>
+    <t>43dd6ee4-4f53-4177-9ad0-9ec9ae7704ca</t>
+  </si>
+  <si>
+    <t>b1488c53-5bdc-4775-be38-4f0c667319bb</t>
+  </si>
+  <si>
+    <t>1d8d13dc-0efc-4190-a159-dcd70644da22</t>
+  </si>
+  <si>
+    <t>报表中心</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop.report</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SYS-MENU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1f635e32-474d-4e93-b497-07063c9272ae</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework.workflow.file-w</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework.workflow.file-w.open</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework.workflow.file-w.approval</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework.workflow.file-w.done</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework.workflow.file-my</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>develop.report.designer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>报表设计器</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yuque</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/report/designer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/framework-workflow/file-my</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework.data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>database</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3fec80da-7c6c-4f8a-a73c-3d37994b8935</t>
+  </si>
+  <si>
+    <t>framework.data.tabular</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>framework.data.category</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/framework-data/tabular</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/framework-data/category</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>zero.data.file-tree</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -747,7 +833,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -770,11 +856,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -837,6 +936,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1156,10 +1258,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3CE16B6-AAB7-164E-9110-1CA8A0C9AC3E}">
-  <dimension ref="A2:L34"/>
+  <dimension ref="A2:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
@@ -1185,16 +1287,16 @@
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
@@ -1387,7 +1489,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>131</v>
+        <v>104</v>
       </c>
       <c r="G9" s="14" t="s">
         <v>29</v>
@@ -1418,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="20" t="s">
-        <v>150</v>
+        <v>117</v>
       </c>
       <c r="G10" s="14" t="s">
         <v>22</v>
@@ -1427,13 +1529,13 @@
         <v>23</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="8" t="s">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="B11" s="8" t="str">
         <f>A$9</f>
@@ -1449,671 +1551,664 @@
         <v>2</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>151</v>
+        <v>118</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>165</v>
+        <v>132</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>153</v>
+        <v>120</v>
       </c>
       <c r="J11" s="9"/>
       <c r="K11" s="10" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="8" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="B12" s="17"/>
       <c r="C12" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="6">
-        <v>5720</v>
+        <v>5890</v>
       </c>
       <c r="E12" s="9">
         <v>1</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>25</v>
+        <v>126</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13" s="17" t="str">
-        <f>A$12</f>
-        <v>66c86ff3-39fe-4fbb-8bb4-8b8977b9745b</v>
-      </c>
-      <c r="C13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="9">
-        <v>1005</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>112</v>
+      <c r="D13" s="6">
+        <v>7000</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>65</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="J13" s="9"/>
+        <v>66</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="8" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B14" s="17" t="str">
-        <f t="shared" ref="B14:B18" si="0">A$12</f>
-        <v>66c86ff3-39fe-4fbb-8bb4-8b8977b9745b</v>
-      </c>
-      <c r="C14" s="14" t="s">
+        <f>A$13</f>
+        <v>d266e5ed-f743-4a8f-bf0c-3f4498fc6fba</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>26</v>
       </c>
       <c r="D14" s="9">
-        <v>1010</v>
-      </c>
-      <c r="E14" s="2">
+        <v>1005</v>
+      </c>
+      <c r="E14" s="23">
         <v>2</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>25</v>
+        <v>110</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" s="17" t="str">
-        <f>A$14</f>
-        <v>fe6e15c5-18b8-403d-a7f3-83c39f36ffc1</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="B15" s="17"/>
       <c r="C15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="9">
-        <v>1005</v>
-      </c>
-      <c r="E15" s="25">
-        <v>3</v>
+      <c r="D15" s="6">
+        <v>7100</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>162</v>
+        <v>75</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>135</v>
+        <v>24</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="8" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="B16" s="17" t="str">
-        <f t="shared" ref="B16:B17" si="1">A$14</f>
-        <v>fe6e15c5-18b8-403d-a7f3-83c39f36ffc1</v>
+        <f>A$15</f>
+        <v>868442e3-2bcf-4549-a1d1-20db042b07d0</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="9">
-        <v>1010</v>
-      </c>
-      <c r="E16" s="25">
-        <v>3</v>
+        <v>1005</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>142</v>
+        <v>83</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>147</v>
+        <v>82</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="8" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B17" s="17" t="str">
-        <f t="shared" si="1"/>
-        <v>fe6e15c5-18b8-403d-a7f3-83c39f36ffc1</v>
+        <f>A$16</f>
+        <v>6ab0911e-be39-435a-a46c-da1a2aa52648</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="9">
-        <v>1015</v>
+        <v>1005</v>
       </c>
       <c r="E17" s="25">
         <v>3</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>164</v>
+        <v>85</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>136</v>
+        <v>87</v>
       </c>
       <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="8" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B18" s="17" t="str">
-        <f t="shared" si="0"/>
-        <v>66c86ff3-39fe-4fbb-8bb4-8b8977b9745b</v>
+        <f>A$15</f>
+        <v>868442e3-2bcf-4549-a1d1-20db042b07d0</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="9">
-        <v>1015</v>
+        <v>1010</v>
       </c>
       <c r="E18" s="2">
         <v>2</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>127</v>
+        <v>62</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>126</v>
+        <v>90</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>128</v>
+        <v>95</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" s="17"/>
+        <v>125</v>
+      </c>
+      <c r="B19" s="17" t="str">
+        <f>A$18</f>
+        <v>d6470316-65ab-4fb3-9d2e-fcfb456259ba</v>
+      </c>
       <c r="C19" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="6">
-        <v>5890</v>
-      </c>
-      <c r="E19" s="9">
-        <v>1</v>
+        <v>77</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1005</v>
+      </c>
+      <c r="E19" s="25">
+        <v>3</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>161</v>
+        <v>121</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>159</v>
+        <v>123</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="6">
-        <v>6000</v>
-      </c>
-      <c r="E20" s="9">
-        <v>1</v>
-      </c>
-      <c r="F20" s="20" t="s">
-        <v>91</v>
+        <v>53</v>
+      </c>
+      <c r="B20" s="17" t="str">
+        <f>A$18</f>
+        <v>d6470316-65ab-4fb3-9d2e-fcfb456259ba</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="9">
+        <v>1010</v>
+      </c>
+      <c r="E20" s="25">
+        <v>3</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>92</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="J20" s="13"/>
+        <v>54</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B21" s="8" t="str">
-        <f t="shared" ref="B21:B22" si="2">A$20</f>
-        <v>c7cfa352-0b7f-4b1d-91ba-8de91468ee4c</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>86</v>
+        <v>56</v>
+      </c>
+      <c r="B21" s="17" t="str">
+        <f t="shared" ref="B21:B22" si="0">A$18</f>
+        <v>d6470316-65ab-4fb3-9d2e-fcfb456259ba</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="D21" s="9">
         <v>1015</v>
       </c>
-      <c r="E21" s="23">
-        <v>2</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>92</v>
+      <c r="E21" s="25">
+        <v>3</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>93</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="I21" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="J21" s="13"/>
+        <v>74</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B22" s="8" t="str">
-        <f t="shared" si="2"/>
-        <v>c7cfa352-0b7f-4b1d-91ba-8de91468ee4c</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="16">
-        <v>1030</v>
-      </c>
-      <c r="E22" s="23">
-        <v>2</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>93</v>
+        <v>58</v>
+      </c>
+      <c r="B22" s="17" t="str">
+        <f t="shared" si="0"/>
+        <v>d6470316-65ab-4fb3-9d2e-fcfb456259ba</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1020</v>
+      </c>
+      <c r="E22" s="25">
+        <v>3</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>94</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="I22" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="J22" s="13"/>
+        <v>60</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="13" t="s">
-        <v>26</v>
+        <v>160</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="14" t="s">
+        <v>137</v>
       </c>
       <c r="D23" s="6">
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="E23" s="9">
         <v>1</v>
       </c>
-      <c r="F23" s="20" t="s">
-        <v>66</v>
+      <c r="F23" s="24" t="s">
+        <v>138</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>81</v>
+        <v>136</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="I23" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="13"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B24" s="8" t="str">
+        <v>161</v>
+      </c>
+      <c r="B24" s="17" t="str">
         <f>A$23</f>
-        <v>d266e5ed-f743-4a8f-bf0c-3f4498fc6fba</v>
+        <v>ab07e5df-94ac-43c0-a66d-55131627ee33</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="D24" s="9">
-        <v>1100</v>
-      </c>
-      <c r="E24" s="2">
+        <v>1005</v>
+      </c>
+      <c r="E24" s="26">
         <v>2</v>
       </c>
-      <c r="F24" s="20" t="s">
-        <v>83</v>
+      <c r="F24" s="24" t="s">
+        <v>141</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="J24" s="13"/>
+        <v>142</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="8" t="s">
-        <v>69</v>
+        <v>162</v>
       </c>
       <c r="B25" s="17" t="str">
-        <f>A$24</f>
-        <v>12b5f844-66b6-4034-b717-9d3224c7fb65</v>
+        <f t="shared" ref="B25:B28" si="1">A$23</f>
+        <v>ab07e5df-94ac-43c0-a66d-55131627ee33</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="D25" s="9">
-        <v>1005</v>
-      </c>
-      <c r="E25" s="25">
-        <v>3</v>
+        <v>1010</v>
+      </c>
+      <c r="E25" s="26">
+        <v>2</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>76</v>
+        <v>143</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="I25" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="13"/>
+        <v>146</v>
+      </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="8" t="s">
-        <v>72</v>
+        <v>163</v>
       </c>
       <c r="B26" s="17" t="str">
-        <f>A$24</f>
-        <v>12b5f844-66b6-4034-b717-9d3224c7fb65</v>
+        <f t="shared" si="1"/>
+        <v>ab07e5df-94ac-43c0-a66d-55131627ee33</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="D26" s="9">
-        <v>1010</v>
-      </c>
-      <c r="E26" s="25">
-        <v>3</v>
+        <v>1015</v>
+      </c>
+      <c r="E26" s="26">
+        <v>2</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>73</v>
+        <v>148</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="13"/>
+        <v>151</v>
+      </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B27" s="17"/>
+        <v>164</v>
+      </c>
+      <c r="B27" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>ab07e5df-94ac-43c0-a66d-55131627ee33</v>
+      </c>
       <c r="C27" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="6">
-        <v>7100</v>
-      </c>
-      <c r="E27" s="9">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1020</v>
+      </c>
+      <c r="E27" s="26">
+        <v>2</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>61</v>
+        <v>152</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>80</v>
+        <v>153</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="13"/>
+        <v>154</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="8" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="B28" s="17" t="str">
-        <f>A$27</f>
-        <v>868442e3-2bcf-4549-a1d1-20db042b07d0</v>
+        <f t="shared" si="1"/>
+        <v>ab07e5df-94ac-43c0-a66d-55131627ee33</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>26</v>
+        <v>137</v>
       </c>
       <c r="D28" s="9">
-        <v>1005</v>
-      </c>
-      <c r="E28" s="2">
+        <v>1025</v>
+      </c>
+      <c r="E28" s="26">
         <v>2</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="H28" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="I28" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="13"/>
+        <v>158</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="17" t="str">
-        <f>A$28</f>
-        <v>6ab0911e-be39-435a-a46c-da1a2aa52648</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B29" s="17"/>
       <c r="C29" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="9">
-        <v>1005</v>
-      </c>
-      <c r="E29" s="25">
-        <v>3</v>
-      </c>
-      <c r="F29" s="24" t="s">
-        <v>108</v>
+        <v>137</v>
+      </c>
+      <c r="D29" s="6">
+        <v>80000</v>
+      </c>
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>167</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>105</v>
+        <v>166</v>
       </c>
       <c r="H29" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="13"/>
+        <v>80</v>
+      </c>
+      <c r="I29" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="13"/>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B30" s="17" t="str">
-        <f>A$27</f>
-        <v>868442e3-2bcf-4549-a1d1-20db042b07d0</v>
+        <v>79</v>
+      </c>
+      <c r="B30" s="8" t="str">
+        <f>A$29</f>
+        <v>c7cfa352-0b7f-4b1d-91ba-8de91468ee4c</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="9">
-        <v>1010</v>
-      </c>
-      <c r="E30" s="2">
+        <v>137</v>
+      </c>
+      <c r="D30" s="16">
+        <v>1030</v>
+      </c>
+      <c r="E30" s="23">
         <v>2</v>
       </c>
-      <c r="F30" s="24" t="s">
-        <v>62</v>
+      <c r="F30" s="20" t="s">
+        <v>175</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>113</v>
+        <v>176</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="I30" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="13"/>
+        <v>177</v>
+      </c>
+      <c r="I30" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="J30" s="13"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B31" s="17" t="str">
-        <f>A$30</f>
-        <v>d6470316-65ab-4fb3-9d2e-fcfb456259ba</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="B31" s="17"/>
       <c r="C31" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="9">
-        <v>1005</v>
-      </c>
-      <c r="E31" s="25">
-        <v>3</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>154</v>
+        <v>168</v>
+      </c>
+      <c r="D31" s="6">
+        <v>91000</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+      <c r="F31" s="20" t="s">
+        <v>180</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>155</v>
+        <v>76</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="I31" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="13"/>
+        <v>181</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="13"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="8" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B32" s="17" t="str">
-        <f>A$30</f>
-        <v>d6470316-65ab-4fb3-9d2e-fcfb456259ba</v>
+        <f>A$31</f>
+        <v>3fec80da-7c6c-4f8a-a73c-3d37994b8935</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="D32" s="9">
-        <v>1010</v>
-      </c>
-      <c r="E32" s="25">
-        <v>3</v>
+        <v>1005</v>
+      </c>
+      <c r="E32" s="23">
+        <v>2</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>115</v>
+        <v>183</v>
       </c>
       <c r="G32" s="14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>55</v>
+        <v>185</v>
       </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
@@ -2121,32 +2216,32 @@
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="8" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="B33" s="17" t="str">
-        <f t="shared" ref="B33:B34" si="3">A$30</f>
-        <v>d6470316-65ab-4fb3-9d2e-fcfb456259ba</v>
+        <f t="shared" ref="B14:B33" si="2">A$31</f>
+        <v>3fec80da-7c6c-4f8a-a73c-3d37994b8935</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>26</v>
+        <v>168</v>
       </c>
       <c r="D33" s="9">
-        <v>1015</v>
-      </c>
-      <c r="E33" s="25">
-        <v>3</v>
+        <v>1010</v>
+      </c>
+      <c r="E33" s="23">
+        <v>2</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>50</v>
+        <v>186</v>
       </c>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
@@ -2154,36 +2249,159 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="17" t="str">
-        <f t="shared" si="3"/>
-        <v>d6470316-65ab-4fb3-9d2e-fcfb456259ba</v>
+        <v>73</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="9">
-        <v>1020</v>
-      </c>
-      <c r="E34" s="25">
-        <v>3</v>
+        <v>168</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1005</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>117</v>
+        <v>170</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="I34" s="21" t="s">
-        <v>132</v>
+        <v>96</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>25</v>
       </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="13"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="17" t="str">
+        <f>A$34</f>
+        <v>66c86ff3-39fe-4fbb-8bb4-8b8977b9745b</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1005</v>
+      </c>
+      <c r="E35" s="25">
+        <v>3</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="J35" s="9"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" s="17" t="str">
+        <f>A$34</f>
+        <v>66c86ff3-39fe-4fbb-8bb4-8b8977b9745b</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" s="9">
+        <v>1010</v>
+      </c>
+      <c r="E36" s="25">
+        <v>3</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I36" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="J36" s="9"/>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="17" t="str">
+        <f>A$34</f>
+        <v>66c86ff3-39fe-4fbb-8bb4-8b8977b9745b</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D37" s="9">
+        <v>1015</v>
+      </c>
+      <c r="E37" s="25">
+        <v>3</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="I37" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="J37" s="9"/>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="17" t="str">
+        <f>A$34</f>
+        <v>66c86ff3-39fe-4fbb-8bb4-8b8977b9745b</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" s="9">
+        <v>1020</v>
+      </c>
+      <c r="E38" s="25">
+        <v>3</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="J38" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>